<commit_message>
updated Farnell order spreadsheet
</commit_message>
<xml_diff>
--- a/doc/PCB/FarnellOrder.xlsx
+++ b/doc/PCB/FarnellOrder.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
     <t>No Switch</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Num I have</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -100,7 +103,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -110,11 +113,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -469,7 +467,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1082,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R106"/>
+  <dimension ref="A1:S106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,7 +1091,7 @@
     <col min="16" max="16" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>[1]BOM!J2</f>
         <v>2320852</v>
@@ -1119,7 +1117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>[1]BOM!J3</f>
         <v>1759265</v>
@@ -1141,7 +1139,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>[1]BOM!J4</f>
         <v>2320829</v>
@@ -1175,7 +1173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>[1]BOM!J5</f>
         <v>2353063</v>
@@ -1213,8 +1211,11 @@
         <f>P4-Q4</f>
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>[1]BOM!J6</f>
         <v>1759246</v>
@@ -1242,15 +1243,18 @@
         <v>47</v>
       </c>
       <c r="P5" s="2">
-        <f t="shared" ref="P5:P43" si="2">ROUNDUP(O5*1.05,0)</f>
+        <f t="shared" ref="P5:P18" si="2">ROUNDUP(O5*1.05,0)</f>
         <v>50</v>
       </c>
       <c r="R5">
         <f t="shared" ref="R5:R18" si="3">P5-Q5</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>[1]BOM!J7</f>
         <v>2320827</v>
@@ -1288,8 +1292,11 @@
         <f t="shared" si="3"/>
         <v>-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>[1]BOM!J8</f>
         <v>9492615</v>
@@ -1327,8 +1334,11 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>[1]BOM!J9</f>
         <v>1635987</v>
@@ -1366,8 +1376,11 @@
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>[1]BOM!J10</f>
         <v>2099243</v>
@@ -1405,8 +1418,11 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>[1]BOM!J11</f>
         <v>2099235</v>
@@ -1444,8 +1460,11 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>[1]BOM!J12</f>
         <v>2099236</v>
@@ -1483,8 +1502,11 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>[1]BOM!J13</f>
         <v>2129087</v>
@@ -1519,8 +1541,11 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>[1]BOM!J14</f>
         <v>2129113</v>
@@ -1558,8 +1583,11 @@
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>[1]BOM!J15</f>
         <v>2129135</v>
@@ -1594,8 +1622,11 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>[1]BOM!J16</f>
         <v>2129375</v>
@@ -1633,8 +1664,11 @@
         <f t="shared" si="3"/>
         <v>-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>[1]BOM!J17</f>
         <v>2129319</v>
@@ -1669,8 +1703,11 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>[1]BOM!J18</f>
         <v>9332391</v>
@@ -1708,8 +1745,11 @@
         <f t="shared" si="3"/>
         <v>-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>[1]BOM!J19</f>
         <v>2129372</v>
@@ -1747,8 +1787,11 @@
         <f t="shared" si="3"/>
         <v>-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>[1]BOM!J20</f>
         <v>2351393</v>
@@ -1770,7 +1813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>[1]BOM!J21</f>
         <v>2129250</v>
@@ -1792,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <f>[1]BOM!J22</f>
         <v>2129329</v>
@@ -1814,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>[1]BOM!J23</f>
         <v>2129417</v>
@@ -1836,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>[1]BOM!J24</f>
         <v>2336778</v>
@@ -1858,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>[1]BOM!J25</f>
         <v>1332158</v>
@@ -1880,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>[1]BOM!J26</f>
         <v>9604367</v>
@@ -1902,7 +1945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>[1]BOM!J27</f>
         <v>1207334</v>
@@ -1924,7 +1967,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>[1]BOM!J28</f>
         <v>2115900</v>
@@ -1946,7 +1989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>[1]BOM!J29</f>
         <v>2067770</v>
@@ -1968,7 +2011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>[1]BOM!J30</f>
         <v>2377152</v>
@@ -1990,7 +2033,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>[1]BOM!J31</f>
         <v>1568026</v>
@@ -2012,7 +2055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="e">
         <f>[1]BOM!J32</f>
         <v>#N/A</v>
@@ -2030,7 +2073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="e">
         <f>[1]BOM!J33</f>
         <v>#N/A</v>

</xml_diff>